<commit_message>
change text value to boolean value quarterly variables
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B58FBE7-7765-A347-A638-66FA4BB09282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="12" windowWidth="16152" windowHeight="10236"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="209">
   <si>
     <t>name</t>
   </si>
@@ -594,9 +600,6 @@
   </si>
   <si>
     <t>isMissing</t>
-  </si>
-  <si>
-    <t>FALSE</t>
   </si>
   <si>
     <t>no</t>
@@ -650,7 +653,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="10"/>
@@ -724,11 +727,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -770,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -802,9 +813,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -836,6 +865,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1011,21 +1058,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D314"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D305" sqref="D305"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="197.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="197.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -3593,21 +3640,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="37.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="64.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="5" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
@@ -3631,11 +3678,11 @@
       <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
@@ -3645,11 +3692,11 @@
       <c r="B3" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>193</v>
+      <c r="C3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
@@ -3659,11 +3706,11 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
@@ -3673,11 +3720,11 @@
       <c r="B5" s="1">
         <v>1</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>193</v>
+      <c r="C5" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
@@ -3687,11 +3734,11 @@
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>193</v>
+      <c r="C6" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
@@ -3701,11 +3748,11 @@
       <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
@@ -3715,11 +3762,11 @@
       <c r="B8" s="1">
         <v>1</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>193</v>
+      <c r="C8" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
@@ -3729,11 +3776,11 @@
       <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
@@ -3743,11 +3790,11 @@
       <c r="B10" s="1">
         <v>1</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>193</v>
+      <c r="C10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
@@ -3757,11 +3804,11 @@
       <c r="B11" s="1">
         <v>2</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>193</v>
+      <c r="C11" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
@@ -3771,11 +3818,11 @@
       <c r="B12" s="1">
         <v>3</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>193</v>
+      <c r="C12" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
@@ -3785,11 +3832,11 @@
       <c r="B13" s="1">
         <v>4</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>193</v>
+      <c r="C13" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
@@ -3799,11 +3846,11 @@
       <c r="B14" s="1">
         <v>5</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>193</v>
+      <c r="C14" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
@@ -3813,11 +3860,11 @@
       <c r="B15" s="1">
         <v>6</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>193</v>
+      <c r="C15" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
@@ -3827,11 +3874,11 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>193</v>
+      <c r="C16" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
@@ -3841,11 +3888,11 @@
       <c r="B17" s="1">
         <v>2</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>193</v>
+      <c r="C17" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
@@ -3855,11 +3902,11 @@
       <c r="B18" s="1">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>193</v>
+      <c r="C18" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
@@ -3869,11 +3916,11 @@
       <c r="B19" s="1">
         <v>4</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>193</v>
+      <c r="C19" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
@@ -3883,11 +3930,11 @@
       <c r="B20" s="1">
         <v>5</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>193</v>
+      <c r="C20" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
@@ -3897,11 +3944,11 @@
       <c r="B21" s="1">
         <v>6</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>193</v>
+      <c r="C21" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
@@ -3911,11 +3958,11 @@
       <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>193</v>
+      <c r="C22" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
@@ -3925,11 +3972,11 @@
       <c r="B23" s="1">
         <v>2</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>193</v>
+      <c r="C23" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
@@ -3939,11 +3986,11 @@
       <c r="B24" s="1">
         <v>3</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>193</v>
+      <c r="C24" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
@@ -3953,11 +4000,11 @@
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>193</v>
+      <c r="C25" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
@@ -3967,11 +4014,11 @@
       <c r="B26" s="1">
         <v>2</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>193</v>
+      <c r="C26" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
@@ -3981,11 +4028,11 @@
       <c r="B27" s="1">
         <v>3</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>193</v>
+      <c r="C27" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
@@ -3995,11 +4042,11 @@
       <c r="B28" s="1">
         <v>4</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>193</v>
+      <c r="C28" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
@@ -4009,11 +4056,11 @@
       <c r="B29" s="1">
         <v>5</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>193</v>
+      <c r="C29" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">

</xml_diff>

<commit_message>
retry for the quarterly variables
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B58FBE7-7765-A347-A638-66FA4BB09282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4902316-EC2B-6743-96AF-7284EA62FDC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
fix(child_id): added meta-vars to dictionaries
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4902316-EC2B-6743-96AF-7284EA62FDC4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF35826-9076-EA4E-BD4A-9DC53B48833B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="218">
   <si>
     <t>name</t>
   </si>
@@ -648,6 +648,33 @@
   </si>
   <si>
     <t>medium-high deprivated</t>
+  </si>
+  <si>
+    <t>child_id</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>Unique number of the child</t>
+  </si>
+  <si>
+    <t>row_id</t>
+  </si>
+  <si>
+    <t>Unique number of the row (to be sure child_id gets persisted</t>
+  </si>
+  <si>
+    <t>age_years</t>
+  </si>
+  <si>
+    <t>Age of the child in years</t>
+  </si>
+  <si>
+    <t>Age of the child in trimesters</t>
+  </si>
+  <si>
+    <t>aqe_quarters</t>
   </si>
 </sst>
 </file>
@@ -665,7 +692,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -676,6 +703,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -715,12 +748,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,11 +1093,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D314"/>
+  <dimension ref="A1:D318"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D305" sqref="D305"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
@@ -1091,91 +1125,89 @@
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>212</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>88</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>108</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>209</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>88</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>109</v>
+        <v>211</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>110</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>217</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>111</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>86</v>
@@ -1184,82 +1216,82 @@
         <v>89</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>86</v>
@@ -1268,12 +1300,12 @@
         <v>91</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>86</v>
@@ -1282,12 +1314,12 @@
         <v>91</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>86</v>
@@ -1296,12 +1328,12 @@
         <v>91</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>86</v>
@@ -1310,12 +1342,12 @@
         <v>91</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>86</v>
@@ -1324,12 +1356,12 @@
         <v>91</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
@@ -1338,12 +1370,12 @@
         <v>91</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>86</v>
@@ -1352,12 +1384,12 @@
         <v>91</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>86</v>
@@ -1366,12 +1398,12 @@
         <v>91</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>86</v>
@@ -1380,12 +1412,12 @@
         <v>91</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>86</v>
@@ -1394,12 +1426,12 @@
         <v>91</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>86</v>
@@ -1408,12 +1440,12 @@
         <v>91</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>86</v>
@@ -1422,124 +1454,124 @@
         <v>91</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>86</v>
@@ -1548,152 +1580,152 @@
         <v>94</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" customHeight="1">
       <c r="A37" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1">
       <c r="A38" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" customHeight="1">
       <c r="A39" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1">
       <c r="A40" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" customHeight="1">
       <c r="A41" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1">
       <c r="A42" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>86</v>
@@ -1702,12 +1734,12 @@
         <v>97</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" customHeight="1">
       <c r="A46" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>86</v>
@@ -1716,12 +1748,12 @@
         <v>97</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>86</v>
@@ -1730,12 +1762,12 @@
         <v>97</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>86</v>
@@ -1744,12 +1776,12 @@
         <v>97</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" customHeight="1">
       <c r="A49" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>86</v>
@@ -1758,12 +1790,12 @@
         <v>97</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" customHeight="1">
       <c r="A50" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>86</v>
@@ -1772,12 +1804,12 @@
         <v>97</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>86</v>
@@ -1786,12 +1818,12 @@
         <v>97</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>86</v>
@@ -1800,222 +1832,222 @@
         <v>97</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" customHeight="1">
       <c r="A53" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" customHeight="1">
       <c r="A61" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" customHeight="1">
       <c r="A62" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" customHeight="1">
       <c r="A63" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>85</v>
@@ -2024,262 +2056,294 @@
         <v>88</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>86</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" customHeight="1">
       <c r="A84" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" customHeight="1">
+      <c r="A85" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" customHeight="1">
+      <c r="A86" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" customHeight="1">
+      <c r="A87" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" customHeight="1">
+      <c r="A88" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C84" s="1" t="s">
+      <c r="B88" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" customHeight="1">
-      <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
-      <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
-    </row>
-    <row r="86" spans="1:4" ht="15" customHeight="1">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-    </row>
-    <row r="87" spans="1:4" ht="15" customHeight="1">
-      <c r="A87" s="4"/>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-    </row>
-    <row r="88" spans="1:4" ht="15" customHeight="1">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-    </row>
     <row r="89" spans="1:4" ht="15" customHeight="1">
-      <c r="A89" s="4"/>
-      <c r="B89" s="4"/>
-      <c r="C89" s="4"/>
-      <c r="D89" s="4"/>
+      <c r="A89" s="3"/>
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" ht="15" customHeight="1">
       <c r="A90" s="4"/>
@@ -3630,6 +3694,30 @@
       <c r="B314" s="4"/>
       <c r="C314" s="4"/>
       <c r="D314" s="4"/>
+    </row>
+    <row r="315" spans="1:4" ht="15" customHeight="1">
+      <c r="A315" s="4"/>
+      <c r="B315" s="4"/>
+      <c r="C315" s="4"/>
+      <c r="D315" s="4"/>
+    </row>
+    <row r="316" spans="1:4" ht="15" customHeight="1">
+      <c r="A316" s="4"/>
+      <c r="B316" s="4"/>
+      <c r="C316" s="4"/>
+      <c r="D316" s="4"/>
+    </row>
+    <row r="317" spans="1:4" ht="15" customHeight="1">
+      <c r="A317" s="4"/>
+      <c r="B317" s="4"/>
+      <c r="C317" s="4"/>
+      <c r="D317" s="4"/>
+    </row>
+    <row r="318" spans="1:4" ht="15" customHeight="1">
+      <c r="A318" s="4"/>
+      <c r="B318" s="4"/>
+      <c r="C318" s="4"/>
+      <c r="D318" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3643,9 +3731,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:C29"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
fix: version stuff and age_quarters instead of aqe_quarters
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF35826-9076-EA4E-BD4A-9DC53B48833B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C326CFF-E925-4448-9C8C-7D54BA905AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -674,7 +674,7 @@
     <t>Age of the child in trimesters</t>
   </si>
   <si>
-    <t>aqe_quarters</t>
+    <t>age_quarters</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1097,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
fix(merged-angela): merged angela's changes into this branch
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
+++ b/R/data/dictionaries/core/1_1/1_1_quarterly_repeated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/core/1_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C326CFF-E925-4448-9C8C-7D54BA905AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FC0896-DD77-0844-AB67-172EEDD0807B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1091,6 +1091,26 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{241614CE-9772-7840-8A90-27420669B396}">
+  <we:reference id="wa104380343" version="2.2.0.0" store="en-001" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa104380343" version="2.2.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D318"/>

</xml_diff>